<commit_message>
Added chapter on univariate eda.
</commit_message>
<xml_diff>
--- a/_book/data/cinnamon_rolls.xlsx
+++ b/_book/data/cinnamon_rolls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilehatch/Dropbox/Teaching/MSB 325/quarto-live/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6BAFD5-6253-AC49-89C7-DDFBD3882D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F22E0C9-F121-364F-98A0-0D0D81E77BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17860" yWindow="4260" windowWidth="32820" windowHeight="28560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,10 +691,10 @@
     <t>{"ImportId":"Q48"}</t>
   </si>
   <si>
-    <t>What do you prefer for on-demand availability in the outside the classroom? (check all that apply)</t>
-  </si>
-  <si>
-    <t>What is the most that you would be willing to pay (in dollars) for a fresh cinnamon roll delivered to the classroom before and after class? - 1</t>
+    <t>What snacks do you prefer for on-demand availability outside your classroom? (check all that apply)</t>
+  </si>
+  <si>
+    <t>What is the most that you would be willing to pay (in dollars) for a fresh cinnamon roll delivered to the classroom before or after class? - 1</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1061,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>